<commit_message>
+ template update fix
</commit_message>
<xml_diff>
--- a/files/templates/QuickConvertTemplate.xlsx
+++ b/files/templates/QuickConvertTemplate.xlsx
@@ -1,38 +1,47 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10315"/>
   <workbookPr dateCompatibility="0" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robalvarez/Desktop/EdTech QTI/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ryanrefugia/Desktop/examHelperQTI/files/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{1D26D9CD-2B66-D542-8D1B-9402C9410F55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{F6161320-B1D1-0041-AF10-7DCE34C2E263}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5180" yWindow="3420" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Blackboard_Quiz_Sample" sheetId="1" r:id="rId1"/>
+    <sheet name="Instructions" sheetId="3" r:id="rId1"/>
+    <sheet name="Questions" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="28" uniqueCount="18">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="64" uniqueCount="53">
   <si>
     <t>MC</t>
   </si>
   <si>
-    <t>Which of the following is a prime number?</t>
-  </si>
-  <si>
     <t>Incorrect</t>
   </si>
   <si>
@@ -42,50 +51,403 @@
     <t>MA</t>
   </si>
   <si>
-    <t>Which of the following numbers is a prime number?</t>
-  </si>
-  <si>
     <t>TF</t>
   </si>
   <si>
-    <t>3 is a prime number.</t>
-  </si>
-  <si>
     <t>ESS</t>
   </si>
   <si>
-    <t>Tell me your life story.</t>
-  </si>
-  <si>
     <t>FIB</t>
   </si>
   <si>
-    <t>Two plus two equals _____.</t>
-  </si>
-  <si>
     <t>four</t>
   </si>
   <si>
-    <t xml:space="preserve"> ____ is the powerhouse of the cell.</t>
-  </si>
-  <si>
     <t>mitochondria</t>
   </si>
   <si>
-    <t>Which of the following is not a prime number?</t>
-  </si>
-  <si>
     <t>incorrect</t>
   </si>
   <si>
     <t>correct</t>
+  </si>
+  <si>
+    <t>REMINDER:</t>
+  </si>
+  <si>
+    <t>HOW TO USE THIS TEMPLATE?</t>
+  </si>
+  <si>
+    <r>
+      <t>• MC (Multiple Choice):</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> For questions that have a single correct answer.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>• MA (Multiple Answer):</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> For questions with more than one correct answer.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>• FIB (Fill in the Blank):</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> For questions where users must supply missing words or phrases.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>• ESS (Essay):</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> For open-ended or essay-type questions that require manual grading.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>• TF (True or False):</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> For statements that are either true or false.</t>
+    </r>
+  </si>
+  <si>
+    <t>HOW TO FORMAT THE QUESTIONS?</t>
+  </si>
+  <si>
+    <t>QUICK CONVERT EXCEL FILE TEMPLATE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WHEN TO USE THE QUICK CONVERT? </t>
+  </si>
+  <si>
+    <t>QUESTION TYPES:</t>
+  </si>
+  <si>
+    <t>All question types are to be input on the QUESTIONS sheet beside this sheet, the INSTRUCTIONS. The first column specifies the exam type, followed by the question and additional columns depending on the type of question.</t>
+  </si>
+  <si>
+    <t>The first column is the exam type (MC/MA). The second column is the question. The following columns are the choices with an adjacent column per choice for "correct"/"incorrect" tagging.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">- </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Column 1:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> MC or MA</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">- </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Column 2:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Question</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">- </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Column 3 onward:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Choice 1, Tag (correct/incorrect), Choice 2, Tag, etc.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">- </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Column 1:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> TF</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">- </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Column 3:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> TRUE or FALSE</t>
+    </r>
+  </si>
+  <si>
+    <t>The first column is the exam type (ESS). The second column is the essay question. No further columns are required.</t>
+  </si>
+  <si>
+    <t>The first column is the exam type (FIB). The second column is the question. The next columns are all possible correct answers.</t>
+  </si>
+  <si>
+    <t>Description: This sheet provides general instructions on how to properly use the template. It explains how to input questions, how to format answers, and how to mark correct responses where applicable. This page helps users understand the rules and standards needed to ensure a successful conversion to QTI.</t>
+  </si>
+  <si>
+    <t>You should use Quick Convert when you want to instantly convert an entire Excel file of questions into a QTI package without selecting specific items.This is ideal when:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     • You are uploading a complete set of exam questions.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     • You want a fast and straightforward conversion process.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     • You don’t need to filter or hand-pick questions, unlike the Item Bank feature.</t>
+  </si>
+  <si>
+    <r>
+      <t>1. Do not modify the template structure</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1" tint="4.9989318521683403E-2"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> – Ensure that all columns and rows remain as formatted.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>2. Fill in the required details</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1" tint="4.9989318521683403E-2"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1" tint="4.9989318521683403E-2"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>– Complete all necessary fields such as the question, choices and correct answers, if required.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>3. Input questions carefully</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1" tint="4.9989318521683403E-2"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> – Ensure accuracy in formatting, grammar, and answer choices.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>4. Use designated answer formats</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1" tint="4.9989318521683403E-2"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> – Multiple-choice, True/False, Fill-in-the-Blanks, and Short Essay formats should follow the provided structure.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>5. Review before finalizing</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1" tint="4.9989318521683403E-2"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> – Double-check all content before submitting or distributing the exam.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">The first column is the exam type (TF). The second column is the statement or question, followed by the correct answer in all caps. </t>
+  </si>
+  <si>
+    <t>(1) MULTIPLE CHOICE (MC) &amp; MULTIPLE ANSWER (MA)</t>
+  </si>
+  <si>
+    <t>(2) TRUE OR FALSE</t>
+  </si>
+  <si>
+    <t>(3) ESSAY</t>
+  </si>
+  <si>
+    <t>(4) FILL IN  THE BLANK</t>
+  </si>
+  <si>
+    <t>[SAMPLE ONLY - REMOVE ] Which of the following is a prime number?</t>
+  </si>
+  <si>
+    <t>[SAMPLE ONLY - REMOVE ] Which of the following numbers is a prime number?</t>
+  </si>
+  <si>
+    <t>[SAMPLE ONLY - REMOVE ]  3 is a prime number.</t>
+  </si>
+  <si>
+    <t>[SAMPLE ONLY - REMOVE ]  Tell me your life story.</t>
+  </si>
+  <si>
+    <t>[SAMPLE ONLY - REMOVE ]  Two plus two equals _____.</t>
+  </si>
+  <si>
+    <t>[SAMPLE ONLY - REMOVE ]  ____ is the powerhouse of the cell.</t>
+  </si>
+  <si>
+    <t>[SAMPLE ONLY - REMOVE ] Which of the following is not a prime number?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -220,8 +582,52 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1" tint="4.9989318521683403E-2"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1" tint="4.9989318521683403E-2"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1" tint="4.9989318521683403E-2"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1" tint="4.9989318521683403E-2"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -401,8 +807,14 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="17">
     <border>
       <start/>
       <end/>
@@ -517,6 +929,99 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <start style="thin">
+        <color indexed="64"/>
+      </start>
+      <end style="thin">
+        <color indexed="64"/>
+      </end>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <start style="thin">
+        <color theme="0"/>
+      </start>
+      <end style="thin">
+        <color theme="0"/>
+      </end>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <start style="thin">
+        <color theme="1"/>
+      </start>
+      <end/>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <start/>
+      <end style="thin">
+        <color theme="0"/>
+      </end>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <start style="thin">
+        <color theme="0"/>
+      </start>
+      <end/>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <start/>
+      <end/>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <start/>
+      <end style="thin">
+        <color theme="1"/>
+      </end>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -562,8 +1067,44 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -938,153 +1479,377 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9E4D0B2-A68F-48E3-861D-AC1107B4C43F}">
+  <dimension ref="A1:N42"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A44" sqref="A44"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="136.1640625" style="3" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="6"/>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12" s="8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A13" s="8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A14" s="8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A15" s="8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A16" s="8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A18" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+      <c r="A19" s="9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A21" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" s="11"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A22" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B22" s="13"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="13"/>
+      <c r="H22" s="13"/>
+      <c r="I22" s="13"/>
+      <c r="J22" s="13"/>
+      <c r="K22" s="13"/>
+      <c r="L22" s="13"/>
+      <c r="M22" s="13"/>
+      <c r="N22" s="14"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A28" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A29" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+      <c r="A30" s="9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A31" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A32" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A34" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A35" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A36" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A37" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A38" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A39" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A40" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A41" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A42" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:N22"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="217" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+    <sheetView zoomScale="150" zoomScaleNormal="107" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="6" style="4" customWidth="1"/>
+    <col min="2" max="2" width="61.33203125" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="11" style="2"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="2">
+        <v>4</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="2">
+        <v>5</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="2">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1">
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" s="2">
+        <v>2</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="2">
+        <v>3</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" s="2">
         <v>4</v>
       </c>
-      <c r="D1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E1">
+      <c r="H2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2" s="2">
         <v>5</v>
       </c>
-      <c r="F1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G1">
+      <c r="J2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="K2" s="2">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="L2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="M2" s="2">
+        <v>7</v>
+      </c>
+      <c r="N2" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C2">
+      <c r="B4" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7" s="2">
+        <v>4</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2">
-        <v>3</v>
-      </c>
-      <c r="F2" t="s">
-        <v>3</v>
-      </c>
-      <c r="G2">
-        <v>4</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="E7" s="2">
+        <v>5</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G7" s="2">
+        <v>6</v>
+      </c>
+      <c r="H7" s="2" t="s">
         <v>2</v>
-      </c>
-      <c r="I2">
-        <v>5</v>
-      </c>
-      <c r="J2" t="s">
-        <v>3</v>
-      </c>
-      <c r="K2">
-        <v>6</v>
-      </c>
-      <c r="L2" t="s">
-        <v>16</v>
-      </c>
-      <c r="M2">
-        <v>7</v>
-      </c>
-      <c r="N2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7">
-        <v>4</v>
-      </c>
-      <c r="D7" t="s">
-        <v>3</v>
-      </c>
-      <c r="E7">
-        <v>5</v>
-      </c>
-      <c r="F7" t="s">
-        <v>2</v>
-      </c>
-      <c r="G7">
-        <v>6</v>
-      </c>
-      <c r="H7" t="s">
-        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>